<commit_message>
Modifique las importaciones de Beneficiarios y apoyos
</commit_message>
<xml_diff>
--- a/Archivos de proyecto/beneficiarios.xlsx
+++ b/Archivos de proyecto/beneficiarios.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="114">
   <si>
     <t>CURP</t>
   </si>
@@ -345,6 +345,27 @@
   </si>
   <si>
     <t>320010017</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>example@hotmail.com</t>
+  </si>
+  <si>
+    <t>Fecha Nacimiento</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>Perfil SocioDemografico</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>Clave Municipio</t>
   </si>
 </sst>
 </file>
@@ -386,16 +407,16 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -451,9 +472,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -477,12 +499,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -762,46 +785,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG12"/>
+  <dimension ref="A1:AM12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AM1" sqref="AM1:AM1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" customWidth="1"/>
-    <col min="13" max="13" width="24.7109375" customWidth="1"/>
-    <col min="14" max="14" width="24.28515625" customWidth="1"/>
-    <col min="15" max="15" width="25.5703125" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.5703125" customWidth="1"/>
-    <col min="22" max="22" width="24.7109375" customWidth="1"/>
-    <col min="23" max="23" width="17.7109375" customWidth="1"/>
-    <col min="24" max="24" width="16.140625" customWidth="1"/>
-    <col min="25" max="25" width="18.28515625" customWidth="1"/>
-    <col min="26" max="26" width="17.42578125" customWidth="1"/>
-    <col min="27" max="27" width="17" customWidth="1"/>
-    <col min="28" max="28" width="16.7109375" customWidth="1"/>
-    <col min="29" max="29" width="17.28515625" customWidth="1"/>
-    <col min="30" max="30" width="17.85546875" customWidth="1"/>
-    <col min="31" max="31" width="15.7109375" customWidth="1"/>
-    <col min="32" max="32" width="15.5703125" customWidth="1"/>
-    <col min="33" max="33" width="18" customWidth="1"/>
+    <col min="3" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" customWidth="1"/>
+    <col min="15" max="15" width="24.28515625" customWidth="1"/>
+    <col min="16" max="16" width="25.5703125" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.5703125" customWidth="1"/>
+    <col min="23" max="23" width="24.7109375" customWidth="1"/>
+    <col min="24" max="24" width="17.7109375" customWidth="1"/>
+    <col min="25" max="25" width="16.140625" customWidth="1"/>
+    <col min="26" max="26" width="18.28515625" customWidth="1"/>
+    <col min="27" max="27" width="17.42578125" customWidth="1"/>
+    <col min="28" max="28" width="17" customWidth="1"/>
+    <col min="29" max="29" width="16.7109375" customWidth="1"/>
+    <col min="30" max="30" width="17.28515625" customWidth="1"/>
+    <col min="31" max="31" width="17.85546875" customWidth="1"/>
+    <col min="32" max="32" width="15.7109375" customWidth="1"/>
+    <col min="33" max="33" width="15.5703125" customWidth="1"/>
+    <col min="34" max="34" width="25.28515625" customWidth="1"/>
+    <col min="35" max="35" width="20.42578125" customWidth="1"/>
+    <col min="36" max="36" width="17.140625" customWidth="1"/>
+    <col min="37" max="37" width="16.140625" customWidth="1"/>
+    <col min="38" max="38" width="23.7109375" customWidth="1"/>
+    <col min="39" max="39" width="18.5703125" customWidth="1"/>
+    <col min="40" max="40" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -901,8 +930,26 @@
       <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="AH1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
@@ -933,7 +980,7 @@
       <c r="J2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>97</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -1002,8 +1049,16 @@
       <c r="AG2" s="4">
         <v>2</v>
       </c>
+      <c r="AH2" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>40</v>
       </c>
@@ -1034,7 +1089,7 @@
       <c r="J3" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="7" t="s">
         <v>98</v>
       </c>
       <c r="L3" s="4" t="s">
@@ -1103,8 +1158,16 @@
       <c r="AG3" s="4">
         <v>2</v>
       </c>
+      <c r="AH3" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
     </row>
-    <row r="4" spans="1:33" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>45</v>
       </c>
@@ -1135,7 +1198,7 @@
       <c r="J4" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="7" t="s">
         <v>99</v>
       </c>
       <c r="L4" s="4" t="s">
@@ -1204,8 +1267,16 @@
       <c r="AG4" s="4">
         <v>2</v>
       </c>
+      <c r="AH4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
     </row>
-    <row r="5" spans="1:33" ht="24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" ht="36" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>51</v>
       </c>
@@ -1236,7 +1307,7 @@
       <c r="J5" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>100</v>
       </c>
       <c r="L5" s="4" t="s">
@@ -1305,8 +1376,16 @@
       <c r="AG5" s="4">
         <v>2</v>
       </c>
+      <c r="AH5" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
     </row>
-    <row r="6" spans="1:33" ht="24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" ht="36" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>58</v>
       </c>
@@ -1337,7 +1416,7 @@
       <c r="J6" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>101</v>
       </c>
       <c r="L6" s="4" t="s">
@@ -1406,8 +1485,16 @@
       <c r="AG6" s="4">
         <v>2</v>
       </c>
+      <c r="AH6" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
     </row>
-    <row r="7" spans="1:33" ht="24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>64</v>
       </c>
@@ -1438,7 +1525,7 @@
       <c r="J7" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="7" t="s">
         <v>102</v>
       </c>
       <c r="L7" s="4" t="s">
@@ -1507,8 +1594,16 @@
       <c r="AG7" s="4">
         <v>2</v>
       </c>
+      <c r="AH7" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
     </row>
-    <row r="8" spans="1:33" ht="24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" ht="48" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>68</v>
       </c>
@@ -1539,7 +1634,7 @@
       <c r="J8" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="7" t="s">
         <v>103</v>
       </c>
       <c r="L8" s="4" t="s">
@@ -1608,8 +1703,16 @@
       <c r="AG8" s="4">
         <v>2</v>
       </c>
+      <c r="AH8" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="4"/>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="4"/>
     </row>
-    <row r="9" spans="1:33" ht="24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" ht="48" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>73</v>
       </c>
@@ -1640,7 +1743,7 @@
       <c r="J9" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="7" t="s">
         <v>104</v>
       </c>
       <c r="L9" s="4" t="s">
@@ -1709,8 +1812,16 @@
       <c r="AG9" s="4">
         <v>2</v>
       </c>
+      <c r="AH9" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="4"/>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="4"/>
     </row>
-    <row r="10" spans="1:33" ht="24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" ht="24" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>79</v>
       </c>
@@ -1741,7 +1852,7 @@
       <c r="J10" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="7" t="s">
         <v>105</v>
       </c>
       <c r="L10" s="4" t="s">
@@ -1810,8 +1921,16 @@
       <c r="AG10" s="4">
         <v>2</v>
       </c>
+      <c r="AH10" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI10" s="4"/>
+      <c r="AJ10" s="4"/>
+      <c r="AK10" s="4"/>
+      <c r="AL10" s="4"/>
+      <c r="AM10" s="4"/>
     </row>
-    <row r="11" spans="1:33" ht="24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" ht="24" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>84</v>
       </c>
@@ -1842,7 +1961,7 @@
       <c r="J11" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="7" t="s">
         <v>106</v>
       </c>
       <c r="L11" s="4" t="s">
@@ -1911,12 +2030,178 @@
       <c r="AG11" s="4">
         <v>2</v>
       </c>
+      <c r="AH11" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI11" s="4"/>
+      <c r="AJ11" s="4"/>
+      <c r="AK11" s="4"/>
+      <c r="AL11" s="4"/>
+      <c r="AM11" s="4"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="K12" s="7"/>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f>A12+1</f>
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <f>B12+1</f>
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:AM12" si="0">C12+1</f>
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="AI12">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="AJ12">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="AK12">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="AL12">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="AM12">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AH2" r:id="rId1"/>
+    <hyperlink ref="AH3:AH11" r:id="rId2" display="example@hotmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>